<commit_message>
Avoid insertion of records if it already has the new items in the Queue to Process
</commit_message>
<xml_diff>
--- a/Data/Transactions.xlsx
+++ b/Data/Transactions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\REFramework\Automate_UIApplication\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{124103C8-D4FA-45B7-B959-483985290EFC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A5ADAB9-7F6F-4AF8-9ECC-513F35A2F7C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="9">
   <si>
     <t>CashIn</t>
   </si>
@@ -45,30 +45,6 @@
     <t>NotOnUsCheck</t>
   </si>
   <si>
-    <t>asd</t>
-  </si>
-  <si>
-    <t>dad</t>
-  </si>
-  <si>
-    <t>gtt</t>
-  </si>
-  <si>
-    <t>gfht</t>
-  </si>
-  <si>
-    <t>gregr</t>
-  </si>
-  <si>
-    <t>egfg</t>
-  </si>
-  <si>
-    <t>scs</t>
-  </si>
-  <si>
-    <t>dsd</t>
-  </si>
-  <si>
     <t>UseCashCount</t>
   </si>
   <si>
@@ -79,6 +55,12 @@
   </si>
   <si>
     <t>Use Amount</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>acc</t>
   </si>
 </sst>
 </file>
@@ -400,7 +382,7 @@
   <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -421,380 +403,280 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="B2" s="1">
-        <v>500</v>
+        <v>510</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
+      <c r="A3" s="1">
+        <v>120</v>
       </c>
       <c r="B3" s="1">
-        <v>510</v>
+        <v>520</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="B4" s="1">
-        <v>520</v>
+        <v>530</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="B5" s="1">
-        <v>530</v>
+        <v>540</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>140</v>
+      <c r="A6" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="B6" s="1">
-        <v>540</v>
+        <v>550</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="B7" s="1">
-        <v>550</v>
+        <v>560</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>4</v>
+      <c r="A8" s="1">
+        <v>170</v>
       </c>
       <c r="B8" s="1">
-        <v>560</v>
+        <v>570</v>
       </c>
       <c r="C8">
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>170</v>
+      <c r="A9" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>570</v>
+        <v>580</v>
       </c>
       <c r="C9">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="B10" s="1">
-        <v>580</v>
+        <v>590</v>
       </c>
       <c r="C10">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="B11" s="1">
-        <v>590</v>
+        <v>600</v>
       </c>
       <c r="C11">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>5</v>
+      <c r="A12" s="1">
+        <v>210</v>
       </c>
       <c r="B12" s="1">
-        <v>600</v>
+        <v>610</v>
       </c>
       <c r="C12">
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="B13" s="1">
-        <v>610</v>
+        <v>620</v>
       </c>
       <c r="C13">
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B14" s="1">
-        <v>620</v>
+        <v>630</v>
       </c>
       <c r="C14">
         <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>7</v>
+      <c r="A15" s="1">
+        <v>240</v>
       </c>
       <c r="B15" s="1">
-        <v>630</v>
+        <v>640</v>
       </c>
       <c r="C15">
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>8</v>
+      <c r="A16" s="1">
+        <v>250</v>
       </c>
       <c r="B16" s="1">
-        <v>640</v>
+        <v>650</v>
       </c>
       <c r="C16">
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
-        <v>170</v>
-      </c>
-      <c r="B17" s="1">
-        <v>650</v>
-      </c>
-      <c r="C17">
-        <v>16</v>
-      </c>
-      <c r="D17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
-        <v>180</v>
-      </c>
-      <c r="B18" s="1">
-        <v>660</v>
-      </c>
-      <c r="C18">
-        <v>17</v>
-      </c>
-      <c r="D18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
-        <v>190</v>
-      </c>
-      <c r="B19" s="1">
-        <v>670</v>
-      </c>
-      <c r="C19">
-        <v>18</v>
-      </c>
-      <c r="D19" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
-        <v>200</v>
-      </c>
-      <c r="B20" s="1">
-        <v>680</v>
-      </c>
-      <c r="C20">
-        <v>19</v>
-      </c>
-      <c r="D20" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="1">
-        <v>690</v>
-      </c>
-      <c r="C21">
-        <v>20</v>
-      </c>
-      <c r="D21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
-        <v>220</v>
-      </c>
-      <c r="B22" s="1">
-        <v>700</v>
-      </c>
-      <c r="C22">
-        <v>21</v>
-      </c>
-      <c r="D22" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" s="1">
-        <v>710</v>
-      </c>
-      <c r="C23">
-        <v>22</v>
-      </c>
-      <c r="D23" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="1">
-        <v>240</v>
-      </c>
-      <c r="B24" s="1">
-        <v>720</v>
-      </c>
-      <c r="C24">
-        <v>23</v>
-      </c>
-      <c r="D24" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="1">
-        <v>250</v>
-      </c>
-      <c r="B25" s="1">
-        <v>730</v>
-      </c>
-      <c r="C25">
-        <v>24</v>
-      </c>
-      <c r="D25" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="1">
-        <v>260</v>
-      </c>
-      <c r="B26" s="1">
-        <v>740</v>
-      </c>
-      <c r="C26">
-        <v>25</v>
-      </c>
-      <c r="D26" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
     </row>

</xml_diff>